<commit_message>
1. Seggerview integrated and compilation errors resolved 2. Created a Separate Patch
</commit_message>
<xml_diff>
--- a/docs/psoc6_pin_mapping.xlsx
+++ b/docs/psoc6_pin_mapping.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Code\generic\sumobot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0AA8F97-0D2B-40FA-A6AE-EF7ECC10BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664C0154-6579-4E4D-A0E4-A86444C6A445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{8AE5DF31-592A-4C82-A27E-93C079319DF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8AE5DF31-592A-4C82-A27E-93C079319DF4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Eval Kit" sheetId="2" r:id="rId1"/>
+    <sheet name="GPIO_List" sheetId="1" r:id="rId2"/>
+    <sheet name="Power Circutry" sheetId="3" r:id="rId3"/>
+    <sheet name="SystemResource" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -830,15 +831,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -851,17 +843,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,15 +889,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>30481</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>363535</xdr:colOff>
+      <xdr:colOff>394015</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>11446</xdr:rowOff>
+      <xdr:rowOff>110506</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -911,8 +912,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1" y="0"/>
-          <a:ext cx="5236524" cy="4177681"/>
+          <a:off x="30481" y="99060"/>
+          <a:ext cx="5240334" cy="4217686"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="5240767" cy="4174037"/>
         </a:xfrm>
@@ -8034,7 +8035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FED30B-00B5-47BA-B571-561397501ED9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -8047,7 +8050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E033C9C-8868-4109-81E3-D57AF52B16CB}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -8088,26 +8091,26 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -8124,13 +8127,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -8138,9 +8141,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
@@ -8300,13 +8303,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -8314,9 +8317,9 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
@@ -8350,13 +8353,13 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -8364,21 +8367,21 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -8386,9 +8389,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="5" t="s">
         <v>59</v>
       </c>
@@ -8408,13 +8411,13 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -8422,21 +8425,21 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="7" t="s">
@@ -8444,21 +8447,21 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -8466,15 +8469,15 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -8493,13 +8496,13 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -8507,21 +8510,21 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -8529,21 +8532,21 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="9"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="7" t="s">
@@ -8551,21 +8554,21 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -8573,9 +8576,9 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="5" t="s">
         <v>83</v>
       </c>
@@ -8623,13 +8626,13 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="13" t="s">
         <v>87</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="7" t="s">
@@ -8637,9 +8640,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="9"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="5" t="s">
         <v>89</v>
       </c>
@@ -8802,7 +8805,7 @@
       <c r="A60" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -8816,7 +8819,7 @@
       <c r="A61" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="10" t="s">
         <v>112</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -8830,7 +8833,7 @@
       <c r="A62" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="10" t="s">
         <v>114</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -8844,7 +8847,7 @@
       <c r="A63" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="10" t="s">
         <v>116</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -8858,7 +8861,7 @@
       <c r="A64" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="11" t="s">
         <v>118</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -8995,7 +8998,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -9037,7 +9040,7 @@
       <c r="C77" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -9098,7 +9101,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="8" t="s">
         <v>144</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -9112,7 +9115,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="12" t="s">
         <v>146</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -9126,7 +9129,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="18" t="s">
+      <c r="A84" s="12" t="s">
         <v>148</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -9140,7 +9143,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="12" t="s">
         <v>150</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -9177,12 +9180,42 @@
       <c r="C87" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="10" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
@@ -9192,36 +9225,6 @@
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9231,7 +9234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CEE8CB-91E9-4AA8-9078-4776D86806A1}">
   <dimension ref="S3:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
@@ -9298,7 +9301,7 @@
       </c>
     </row>
     <row r="11" spans="19:21" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S11" s="18" t="s">
+      <c r="S11" s="12" t="s">
         <v>170</v>
       </c>
       <c r="T11" s="4" t="s">
@@ -9309,7 +9312,7 @@
       </c>
     </row>
     <row r="12" spans="19:21" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S12" s="18" t="s">
+      <c r="S12" s="12" t="s">
         <v>173</v>
       </c>
       <c r="T12" s="4" t="s">
@@ -9320,7 +9323,7 @@
       </c>
     </row>
     <row r="13" spans="19:21" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S13" s="18" t="s">
+      <c r="S13" s="12" t="s">
         <v>175</v>
       </c>
       <c r="T13" s="4" t="s">
@@ -9337,4 +9340,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F29FB88-C462-4A47-8B7E-AAC6D4068C3A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>